<commit_message>
Yield file that contains blocks
</commit_message>
<xml_diff>
--- a/_data/2021 Yield.xlsx
+++ b/_data/2021 Yield.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,13 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
   <si>
     <t>Plot Number</t>
   </si>
@@ -118,13 +118,16 @@
   </si>
   <si>
     <t>CC + 60ISC</t>
+  </si>
+  <si>
+    <t>Block</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +139,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,32 +187,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -240,7 +232,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="44511.352121759257" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="36">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E37" sheet="Data"/>
+    <worksheetSource ref="A1:F37" sheet="Data" r:id="rId2"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Plot Number" numFmtId="0">
@@ -538,7 +530,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -614,49 +606,49 @@
     <dataField name="Average of Yield (avg; bu/ac)" fld="3" subtotal="average" baseField="1" baseItem="0"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="13">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -960,754 +952,865 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="30.5703125" style="1" customWidth="1"/>
+    <col min="1" max="7" width="30.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>75.328417551925781</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>77.482015874168184</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>232.17328062804069</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>3.1</v>
+      <c r="B5" s="7">
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>3.1</v>
       </c>
       <c r="D5" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="E5" s="1">
         <v>231.64585471030517</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>4.0999999999999996</v>
+      <c r="B6" s="7">
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="D6" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E6" s="1">
         <v>208.94051923927464</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>3.2</v>
+      <c r="B7" s="7">
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>3.2</v>
       </c>
       <c r="D7" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="E7" s="1">
         <v>223.98853140203451</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="7">
         <v>3</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>75.667936067755591</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>5</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>71.839369630973977</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>5</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>72.610891663641866</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="7">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>69.045749562411771</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>2</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>237.6839887218045</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>5</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>229.93327001326847</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
-        <v>4.2</v>
+      <c r="B14" s="7">
+        <v>2</v>
       </c>
       <c r="C14" s="1">
         <v>4.2</v>
       </c>
       <c r="D14" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="E14" s="1">
         <v>179.6387754312251</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="7">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>6</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>239.97312472357365</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="7">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>70.358940431538613</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="7">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>6</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>73.635658318209309</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>214.63579842989827</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
-        <v>3.1</v>
+      <c r="B19" s="7">
+        <v>1</v>
       </c>
       <c r="C19" s="1">
         <v>3.1</v>
       </c>
       <c r="D19" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="E19" s="1">
         <v>225.74481932773108</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>5</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>71.404874289171204</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>6</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>74.278301520467835</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
-        <v>4.0999999999999996</v>
+      <c r="B22" s="7">
+        <v>1</v>
       </c>
       <c r="C22" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="D22" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E22" s="1">
         <v>212.61343432109689</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
-        <v>4.2</v>
+      <c r="B23" s="7">
+        <v>1</v>
       </c>
       <c r="C23" s="1">
         <v>4.2</v>
       </c>
       <c r="D23" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="E23" s="1">
         <v>174.9558951791243</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="7">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>235.87814241486069</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="7">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>221.98222091994694</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="7">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>6</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>242.69053582485625</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
-        <v>4.0999999999999996</v>
+      <c r="B27" s="7">
+        <v>3</v>
       </c>
       <c r="C27" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="D27" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E27" s="1">
         <v>224.55381026094651</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>2</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>242.05453781512605</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>218.43057098628927</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>68.365014817503535</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>2</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>74.375402395644301</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>6</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>241.9812790800531</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
-        <v>3.2</v>
+      <c r="B33" s="7">
+        <v>1</v>
       </c>
       <c r="C33" s="1">
         <v>3.2</v>
       </c>
       <c r="D33" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="E33" s="1">
         <v>214.28280473241929</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
-        <v>3.1</v>
+      <c r="B34" s="7">
+        <v>3</v>
       </c>
       <c r="C34" s="1">
         <v>3.1</v>
       </c>
       <c r="D34" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="E34" s="1">
         <v>226.95474878372403</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="7">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>5</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>226.56365280849184</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
-        <v>4.2</v>
+      <c r="B36" s="7">
+        <v>3</v>
       </c>
       <c r="C36" s="1">
         <v>4.2</v>
       </c>
       <c r="D36" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="E36" s="1">
         <v>174.58642337461299</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
-        <v>3.2</v>
+      <c r="B37" s="7">
+        <v>3</v>
       </c>
       <c r="C37" s="1">
         <v>3.2</v>
       </c>
       <c r="D37" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="E37" s="1">
         <v>233.15335216718265</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>